<commit_message>
made separate submission script
</commit_message>
<xml_diff>
--- a/EDA/srch_id_1.xlsx
+++ b/EDA/srch_id_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c98b824bff33be6/MSc. Artificial Intelligence VU/MSc. AI Year 1/Data Mining Techniques/Assignment 2/new_clone/dmt-2/EDA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_371659DFFD9C91DE04170B1633B47FB0603A2163" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46ABACB1-0A4B-4ECA-8B8C-4909646E55A1}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_371659DF44BC10E5DA170B6CA376D07750523176" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{639E8656-96A6-44BC-8BAB-A9F4622CF603}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1812" yWindow="1812" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="new_sheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="51">
   <si>
     <t>srch_id</t>
   </si>
@@ -64,9 +64,6 @@
     <t>prop_log_historical_price</t>
   </si>
   <si>
-    <t>position</t>
-  </si>
-  <si>
     <t>price_usd</t>
   </si>
   <si>
@@ -175,16 +172,7 @@
     <t>comp8_rate_percent_diff</t>
   </si>
   <si>
-    <t>click_bool</t>
-  </si>
-  <si>
-    <t>gross_bookings_usd</t>
-  </si>
-  <si>
-    <t>booking_bool</t>
-  </si>
-  <si>
-    <t>2013-04-04 08:32:15</t>
+    <t>2013-02-02 15:27:40</t>
   </si>
 </sst>
 </file>
@@ -586,71 +574,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BC29"/>
+  <dimension ref="A1:AY30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
-      <selection activeCell="BA8" sqref="BA8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13:K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -801,124 +736,79 @@
       <c r="AY1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>50</v>
       </c>
-      <c r="BA1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BB1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>54</v>
-      </c>
       <c r="D2">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E2">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="H2">
         <v>219</v>
       </c>
       <c r="I2">
-        <v>893</v>
+        <v>3180</v>
       </c>
       <c r="J2">
         <v>3</v>
       </c>
       <c r="K2">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="L2">
         <v>1</v>
       </c>
       <c r="M2">
-        <v>2.83</v>
+        <v>2.94</v>
       </c>
       <c r="N2">
-        <v>4.3799999999999999E-2</v>
+        <v>6.9099999999999995E-2</v>
       </c>
       <c r="O2">
-        <v>4.95</v>
+        <v>5.03</v>
       </c>
       <c r="P2">
-        <v>27</v>
+        <v>119</v>
       </c>
       <c r="Q2">
-        <v>104.77</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>19222</v>
       </c>
       <c r="S2">
-        <v>23246</v>
+        <v>1</v>
       </c>
       <c r="T2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X2">
-        <v>1</v>
-      </c>
-      <c r="Y2">
-        <v>1</v>
-      </c>
-      <c r="AB2">
-        <v>1</v>
-      </c>
-      <c r="AF2">
-        <v>0</v>
-      </c>
-      <c r="AG2">
-        <v>0</v>
-      </c>
-      <c r="AI2">
-        <v>0</v>
-      </c>
-      <c r="AJ2">
-        <v>0</v>
-      </c>
-      <c r="AO2">
-        <v>0</v>
-      </c>
-      <c r="AP2">
-        <v>0</v>
-      </c>
-      <c r="AX2">
-        <v>0</v>
-      </c>
-      <c r="AY2">
-        <v>0</v>
-      </c>
-      <c r="BA2">
-        <v>0</v>
-      </c>
-      <c r="BC2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -926,97 +816,76 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D3">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E3">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="H3">
         <v>219</v>
       </c>
       <c r="I3">
-        <v>10404</v>
+        <v>5543</v>
       </c>
       <c r="J3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K3">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="L3">
         <v>1</v>
       </c>
       <c r="M3">
-        <v>2.2000000000000002</v>
+        <v>2.64</v>
       </c>
       <c r="N3">
-        <v>1.49E-2</v>
+        <v>8.43E-2</v>
       </c>
       <c r="O3">
-        <v>5.03</v>
+        <v>4.93</v>
       </c>
       <c r="P3">
-        <v>26</v>
+        <v>118</v>
       </c>
       <c r="Q3">
-        <v>170.74</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>19222</v>
       </c>
       <c r="S3">
-        <v>23246</v>
+        <v>1</v>
       </c>
       <c r="T3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X3">
-        <v>1</v>
-      </c>
-      <c r="Y3">
-        <v>1</v>
-      </c>
-      <c r="AB3">
-        <v>1</v>
-      </c>
-      <c r="AI3">
-        <v>0</v>
-      </c>
-      <c r="AJ3">
-        <v>0</v>
-      </c>
-      <c r="AO3">
-        <v>0</v>
-      </c>
-      <c r="AP3">
-        <v>1</v>
-      </c>
-      <c r="AX3">
-        <v>0</v>
-      </c>
-      <c r="AY3">
-        <v>0</v>
-      </c>
-      <c r="BA3">
-        <v>0</v>
-      </c>
-      <c r="BC3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1024,103 +893,85 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D4">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E4">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="H4">
         <v>219</v>
       </c>
       <c r="I4">
-        <v>21315</v>
+        <v>14142</v>
       </c>
       <c r="J4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K4">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="L4">
         <v>1</v>
       </c>
       <c r="M4">
-        <v>2.2000000000000002</v>
+        <v>2.71</v>
       </c>
       <c r="N4">
-        <v>2.4500000000000001E-2</v>
+        <v>5.5599999999999997E-2</v>
       </c>
       <c r="O4">
-        <v>4.92</v>
+        <v>4.16</v>
       </c>
       <c r="P4">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="Q4">
-        <v>179.8</v>
+        <v>0</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>19222</v>
       </c>
       <c r="S4">
-        <v>23246</v>
+        <v>1</v>
       </c>
       <c r="T4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X4">
-        <v>1</v>
-      </c>
-      <c r="Y4">
-        <v>1</v>
-      </c>
-      <c r="AB4">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
       </c>
       <c r="AF4">
         <v>0</v>
       </c>
-      <c r="AG4">
-        <v>0</v>
-      </c>
-      <c r="AI4">
-        <v>0</v>
-      </c>
-      <c r="AJ4">
-        <v>0</v>
+      <c r="AN4">
+        <v>1</v>
       </c>
       <c r="AO4">
         <v>0</v>
       </c>
       <c r="AP4">
-        <v>0</v>
-      </c>
-      <c r="AX4">
-        <v>0</v>
-      </c>
-      <c r="AY4">
-        <v>0</v>
-      </c>
-      <c r="BA4">
-        <v>0</v>
-      </c>
-      <c r="BC4">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1128,112 +979,82 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D5">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E5">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="H5">
         <v>219</v>
       </c>
       <c r="I5">
-        <v>27348</v>
+        <v>22393</v>
       </c>
       <c r="J5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K5">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="L5">
         <v>1</v>
       </c>
       <c r="M5">
-        <v>2.83</v>
+        <v>2.4</v>
       </c>
       <c r="N5">
-        <v>1.2500000000000001E-2</v>
+        <v>5.6099999999999997E-2</v>
       </c>
       <c r="O5">
-        <v>4.3899999999999997</v>
+        <v>5.03</v>
       </c>
       <c r="P5">
-        <v>34</v>
+        <v>143</v>
       </c>
       <c r="Q5">
-        <v>602.77</v>
+        <v>0</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>19222</v>
       </c>
       <c r="S5">
-        <v>23246</v>
+        <v>1</v>
       </c>
       <c r="T5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X5">
-        <v>1</v>
-      </c>
-      <c r="Y5">
-        <v>1</v>
-      </c>
-      <c r="AB5">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
       </c>
       <c r="AF5">
-        <v>-1</v>
-      </c>
-      <c r="AG5">
-        <v>0</v>
-      </c>
-      <c r="AH5">
-        <v>5</v>
-      </c>
-      <c r="AI5">
-        <v>-1</v>
-      </c>
-      <c r="AJ5">
-        <v>0</v>
-      </c>
-      <c r="AK5">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="AN5">
+        <v>0</v>
       </c>
       <c r="AO5">
         <v>0</v>
       </c>
-      <c r="AP5">
-        <v>1</v>
-      </c>
-      <c r="AX5">
-        <v>-1</v>
-      </c>
-      <c r="AY5">
-        <v>0</v>
-      </c>
-      <c r="AZ5">
-        <v>5</v>
-      </c>
-      <c r="BA5">
-        <v>0</v>
-      </c>
-      <c r="BC5">
-        <v>0</v>
-      </c>
     </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1241,103 +1062,82 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D6">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E6">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="H6">
         <v>219</v>
       </c>
       <c r="I6">
-        <v>29604</v>
+        <v>24194</v>
       </c>
       <c r="J6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K6">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="L6">
         <v>1</v>
       </c>
       <c r="M6">
-        <v>2.64</v>
+        <v>2.94</v>
       </c>
       <c r="N6">
-        <v>0.1241</v>
+        <v>0.20899999999999999</v>
       </c>
       <c r="O6">
-        <v>4.93</v>
+        <v>4.72</v>
       </c>
       <c r="P6">
-        <v>4</v>
+        <v>79</v>
       </c>
       <c r="Q6">
-        <v>143.58000000000001</v>
+        <v>0</v>
       </c>
       <c r="R6">
-        <v>0</v>
+        <v>19222</v>
       </c>
       <c r="S6">
-        <v>23246</v>
+        <v>1</v>
       </c>
       <c r="T6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X6">
-        <v>1</v>
-      </c>
-      <c r="Y6">
-        <v>1</v>
-      </c>
-      <c r="AB6">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <v>0</v>
       </c>
       <c r="AF6">
         <v>0</v>
       </c>
-      <c r="AG6">
-        <v>0</v>
-      </c>
-      <c r="AI6">
-        <v>0</v>
-      </c>
-      <c r="AJ6">
+      <c r="AN6">
         <v>0</v>
       </c>
       <c r="AO6">
         <v>0</v>
       </c>
-      <c r="AP6">
-        <v>0</v>
-      </c>
-      <c r="AX6">
-        <v>0</v>
-      </c>
-      <c r="AY6">
-        <v>0</v>
-      </c>
-      <c r="BA6">
-        <v>0</v>
-      </c>
-      <c r="BC6">
-        <v>0</v>
-      </c>
     </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1345,22 +1145,22 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D7">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E7">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="H7">
         <v>219</v>
       </c>
       <c r="I7">
-        <v>30184</v>
+        <v>28181</v>
       </c>
       <c r="J7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K7">
         <v>4.5</v>
@@ -1369,79 +1169,46 @@
         <v>1</v>
       </c>
       <c r="M7">
-        <v>2.77</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="N7">
-        <v>0.13020000000000001</v>
+        <v>0.18260000000000001</v>
       </c>
       <c r="O7">
-        <v>5.2</v>
+        <v>4.68</v>
       </c>
       <c r="P7">
-        <v>7</v>
+        <v>84.15</v>
       </c>
       <c r="Q7">
-        <v>195.32</v>
+        <v>0</v>
       </c>
       <c r="R7">
-        <v>0</v>
+        <v>19222</v>
       </c>
       <c r="S7">
-        <v>23246</v>
+        <v>1</v>
       </c>
       <c r="T7">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V7">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X7">
-        <v>1</v>
-      </c>
-      <c r="Y7">
-        <v>1</v>
-      </c>
-      <c r="AB7">
-        <v>1</v>
-      </c>
-      <c r="AI7">
-        <v>0</v>
-      </c>
-      <c r="AJ7">
-        <v>0</v>
-      </c>
-      <c r="AK7">
-        <v>7</v>
-      </c>
-      <c r="AO7">
-        <v>0</v>
-      </c>
-      <c r="AP7">
-        <v>0</v>
-      </c>
-      <c r="AX7">
-        <v>0</v>
-      </c>
-      <c r="AY7">
-        <v>0</v>
-      </c>
-      <c r="AZ7">
-        <v>7</v>
-      </c>
-      <c r="BA7">
-        <v>0</v>
-      </c>
-      <c r="BC7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1449,97 +1216,88 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D8">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E8">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="H8">
         <v>219</v>
       </c>
       <c r="I8">
-        <v>44147</v>
+        <v>34263</v>
       </c>
       <c r="J8">
         <v>3</v>
       </c>
       <c r="K8">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="L8">
         <v>1</v>
       </c>
       <c r="M8">
-        <v>2.2000000000000002</v>
+        <v>3.09</v>
       </c>
       <c r="N8">
-        <v>3.56E-2</v>
+        <v>0.13</v>
       </c>
       <c r="O8">
-        <v>4.8099999999999996</v>
+        <v>4.63</v>
       </c>
       <c r="P8">
-        <v>18</v>
+        <v>79</v>
       </c>
       <c r="Q8">
-        <v>129.35</v>
+        <v>0</v>
       </c>
       <c r="R8">
-        <v>0</v>
+        <v>19222</v>
       </c>
       <c r="S8">
-        <v>23246</v>
+        <v>1</v>
       </c>
       <c r="T8">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X8">
-        <v>1</v>
-      </c>
-      <c r="Y8">
-        <v>1</v>
-      </c>
-      <c r="AB8">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <v>0</v>
       </c>
       <c r="AF8">
         <v>0</v>
       </c>
       <c r="AG8">
-        <v>0</v>
-      </c>
-      <c r="AI8">
-        <v>0</v>
-      </c>
-      <c r="AJ8">
-        <v>0</v>
-      </c>
-      <c r="AX8">
-        <v>0</v>
-      </c>
-      <c r="AY8">
-        <v>0</v>
-      </c>
-      <c r="BA8">
-        <v>0</v>
-      </c>
-      <c r="BC8">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="AN8">
+        <v>0</v>
+      </c>
+      <c r="AO8">
+        <v>0</v>
+      </c>
+      <c r="AP8">
+        <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1547,76 +1305,88 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D9">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E9">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="H9">
         <v>219</v>
       </c>
       <c r="I9">
-        <v>50984</v>
+        <v>37567</v>
       </c>
       <c r="J9">
         <v>2</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
-        <v>1.61</v>
+        <v>2.83</v>
+      </c>
+      <c r="N9">
+        <v>1.38E-2</v>
       </c>
       <c r="O9">
-        <v>4.1399999999999997</v>
+        <v>4.21</v>
       </c>
       <c r="P9">
-        <v>35</v>
+        <v>52.4</v>
       </c>
       <c r="Q9">
-        <v>85.37</v>
+        <v>1</v>
       </c>
       <c r="R9">
-        <v>0</v>
+        <v>19222</v>
       </c>
       <c r="S9">
-        <v>23246</v>
+        <v>1</v>
       </c>
       <c r="T9">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X9">
-        <v>1</v>
-      </c>
-      <c r="Y9">
-        <v>1</v>
-      </c>
-      <c r="AB9">
-        <v>1</v>
-      </c>
-      <c r="BA9">
-        <v>0</v>
-      </c>
-      <c r="BC9">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <v>1</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <v>11</v>
+      </c>
+      <c r="AN9">
+        <v>1</v>
+      </c>
+      <c r="AO9">
+        <v>0</v>
+      </c>
+      <c r="AP9">
+        <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1624,100 +1394,85 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D10">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E10">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="H10">
         <v>219</v>
       </c>
       <c r="I10">
-        <v>53341</v>
+        <v>50162</v>
       </c>
       <c r="J10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K10">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="L10">
         <v>1</v>
       </c>
       <c r="M10">
-        <v>2.56</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="N10">
-        <v>0.12379999999999999</v>
+        <v>8.0799999999999997E-2</v>
       </c>
       <c r="O10">
-        <v>5.18</v>
+        <v>4.3600000000000003</v>
       </c>
       <c r="P10">
-        <v>3</v>
+        <v>49.99</v>
       </c>
       <c r="Q10">
-        <v>150.05000000000001</v>
+        <v>1</v>
       </c>
       <c r="R10">
-        <v>0</v>
+        <v>19222</v>
       </c>
       <c r="S10">
-        <v>23246</v>
+        <v>1</v>
       </c>
       <c r="T10">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V10">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X10">
-        <v>1</v>
-      </c>
-      <c r="Y10">
-        <v>1</v>
-      </c>
-      <c r="AB10">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>-1</v>
       </c>
       <c r="AF10">
         <v>0</v>
       </c>
       <c r="AG10">
-        <v>0</v>
-      </c>
-      <c r="AI10">
-        <v>0</v>
-      </c>
-      <c r="AJ10">
-        <v>0</v>
-      </c>
-      <c r="AX10">
-        <v>0</v>
-      </c>
-      <c r="AY10">
-        <v>0</v>
-      </c>
-      <c r="AZ10">
-        <v>6</v>
-      </c>
-      <c r="BA10">
-        <v>0</v>
-      </c>
-      <c r="BC10">
+        <v>10</v>
+      </c>
+      <c r="AN10">
+        <v>0</v>
+      </c>
+      <c r="AO10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1725,22 +1480,22 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D11">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E11">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="H11">
         <v>219</v>
       </c>
       <c r="I11">
-        <v>56880</v>
+        <v>54937</v>
       </c>
       <c r="J11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K11">
         <v>4</v>
@@ -1749,79 +1504,52 @@
         <v>1</v>
       </c>
       <c r="M11">
-        <v>2.83</v>
+        <v>2.08</v>
       </c>
       <c r="N11">
-        <v>0.1028</v>
+        <v>0.16489999999999999</v>
       </c>
       <c r="O11">
-        <v>5.15</v>
+        <v>4.75</v>
       </c>
       <c r="P11">
-        <v>10</v>
+        <v>83.3</v>
       </c>
       <c r="Q11">
-        <v>280.69</v>
+        <v>1</v>
       </c>
       <c r="R11">
-        <v>0</v>
+        <v>19222</v>
       </c>
       <c r="S11">
-        <v>23246</v>
+        <v>1</v>
       </c>
       <c r="T11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V11">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X11">
-        <v>1</v>
-      </c>
-      <c r="Y11">
-        <v>1</v>
-      </c>
-      <c r="AB11">
-        <v>1</v>
-      </c>
-      <c r="AF11">
-        <v>0</v>
-      </c>
-      <c r="AG11">
-        <v>0</v>
-      </c>
-      <c r="AI11">
-        <v>0</v>
-      </c>
-      <c r="AJ11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AN11">
         <v>0</v>
       </c>
       <c r="AO11">
         <v>0</v>
       </c>
-      <c r="AP11">
-        <v>0</v>
-      </c>
-      <c r="AX11">
-        <v>0</v>
-      </c>
-      <c r="AY11">
-        <v>0</v>
-      </c>
-      <c r="BA11">
-        <v>0</v>
-      </c>
-      <c r="BC11">
-        <v>0</v>
-      </c>
     </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1829,97 +1557,73 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D12">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E12">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="H12">
         <v>219</v>
       </c>
       <c r="I12">
-        <v>59267</v>
+        <v>56050</v>
       </c>
       <c r="J12">
         <v>3</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L12">
         <v>1</v>
       </c>
       <c r="M12">
-        <v>2.2000000000000002</v>
+        <v>2.77</v>
+      </c>
+      <c r="N12">
+        <v>0.121</v>
       </c>
       <c r="O12">
-        <v>5.08</v>
+        <v>4.59</v>
       </c>
       <c r="P12">
-        <v>20</v>
+        <v>145</v>
       </c>
       <c r="Q12">
-        <v>190.14</v>
+        <v>0</v>
       </c>
       <c r="R12">
-        <v>0</v>
+        <v>19222</v>
       </c>
       <c r="S12">
-        <v>23246</v>
+        <v>1</v>
       </c>
       <c r="T12">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X12">
-        <v>1</v>
-      </c>
-      <c r="Y12">
-        <v>1</v>
-      </c>
-      <c r="AB12">
-        <v>1</v>
-      </c>
-      <c r="AF12">
-        <v>1</v>
-      </c>
-      <c r="AG12">
-        <v>0</v>
-      </c>
-      <c r="AH12">
-        <v>11</v>
-      </c>
-      <c r="AI12">
-        <v>0</v>
-      </c>
-      <c r="AJ12">
-        <v>0</v>
-      </c>
-      <c r="AX12">
-        <v>0</v>
-      </c>
-      <c r="AY12">
-        <v>0</v>
-      </c>
-      <c r="BA12">
-        <v>0</v>
-      </c>
-      <c r="BC12">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AO12">
+        <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1927,103 +1631,79 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D13">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E13">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="H13">
         <v>219</v>
       </c>
       <c r="I13">
-        <v>59526</v>
+        <v>61632</v>
       </c>
       <c r="J13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K13">
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13">
-        <v>2.2000000000000002</v>
+        <v>3.04</v>
       </c>
       <c r="N13">
-        <v>3.7699999999999997E-2</v>
+        <v>1.3599999999999999E-2</v>
       </c>
       <c r="O13">
-        <v>4.78</v>
+        <v>4.62</v>
       </c>
       <c r="P13">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="Q13">
-        <v>100.89</v>
+        <v>0</v>
       </c>
       <c r="R13">
-        <v>0</v>
+        <v>19222</v>
       </c>
       <c r="S13">
-        <v>23246</v>
+        <v>1</v>
       </c>
       <c r="T13">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V13">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X13">
-        <v>1</v>
-      </c>
-      <c r="Y13">
-        <v>1</v>
-      </c>
-      <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AA13">
+        <v>0</v>
+      </c>
+      <c r="AE13">
         <v>1</v>
       </c>
       <c r="AF13">
         <v>0</v>
       </c>
       <c r="AG13">
-        <v>0</v>
-      </c>
-      <c r="AI13">
-        <v>-1</v>
-      </c>
-      <c r="AJ13">
-        <v>0</v>
-      </c>
-      <c r="AK13">
-        <v>5</v>
-      </c>
-      <c r="AX13">
-        <v>1</v>
-      </c>
-      <c r="AY13">
-        <v>0</v>
-      </c>
-      <c r="AZ13">
-        <v>31</v>
-      </c>
-      <c r="BA13">
-        <v>0</v>
-      </c>
-      <c r="BC13">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2031,112 +1711,76 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D14">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E14">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="H14">
         <v>219</v>
       </c>
       <c r="I14">
-        <v>68914</v>
+        <v>61934</v>
       </c>
       <c r="J14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K14">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="L14">
         <v>1</v>
       </c>
       <c r="M14">
-        <v>2.2000000000000002</v>
+        <v>2.89</v>
       </c>
       <c r="N14">
-        <v>2.06E-2</v>
+        <v>0.24249999999999999</v>
       </c>
       <c r="O14">
-        <v>4.4400000000000004</v>
+        <v>4.6900000000000004</v>
       </c>
       <c r="P14">
-        <v>13</v>
+        <v>88.88</v>
       </c>
       <c r="Q14">
-        <v>100.89</v>
+        <v>1</v>
       </c>
       <c r="R14">
-        <v>0</v>
+        <v>19222</v>
       </c>
       <c r="S14">
-        <v>23246</v>
+        <v>1</v>
       </c>
       <c r="T14">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X14">
-        <v>1</v>
-      </c>
-      <c r="Y14">
-        <v>1</v>
-      </c>
-      <c r="AB14">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AA14">
+        <v>0</v>
+      </c>
+      <c r="AE14">
+        <v>0</v>
       </c>
       <c r="AF14">
         <v>0</v>
       </c>
-      <c r="AG14">
-        <v>0</v>
-      </c>
-      <c r="AH14">
-        <v>11</v>
-      </c>
-      <c r="AI14">
-        <v>0</v>
-      </c>
-      <c r="AJ14">
-        <v>0</v>
-      </c>
-      <c r="AO14">
-        <v>0</v>
-      </c>
-      <c r="AP14">
-        <v>-1</v>
-      </c>
-      <c r="AX14">
-        <v>0</v>
-      </c>
-      <c r="AY14">
-        <v>0</v>
-      </c>
-      <c r="AZ14">
-        <v>11</v>
-      </c>
-      <c r="BA14">
-        <v>1</v>
-      </c>
-      <c r="BB14">
-        <v>114.29</v>
-      </c>
-      <c r="BC14">
-        <v>1</v>
-      </c>
     </row>
-    <row r="15" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2144,19 +1788,19 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D15">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E15">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="H15">
         <v>219</v>
       </c>
       <c r="I15">
-        <v>74474</v>
+        <v>63894</v>
       </c>
       <c r="J15">
         <v>3</v>
@@ -2168,79 +1812,58 @@
         <v>1</v>
       </c>
       <c r="M15">
-        <v>2.4</v>
+        <v>2.77</v>
       </c>
       <c r="N15">
-        <v>0.1255</v>
+        <v>0.2261</v>
       </c>
       <c r="O15">
-        <v>5.03</v>
+        <v>4.88</v>
       </c>
       <c r="P15">
-        <v>2</v>
+        <v>103.98</v>
       </c>
       <c r="Q15">
-        <v>210.84</v>
+        <v>0</v>
       </c>
       <c r="R15">
-        <v>0</v>
+        <v>19222</v>
       </c>
       <c r="S15">
-        <v>23246</v>
+        <v>1</v>
       </c>
       <c r="T15">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V15">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X15">
-        <v>1</v>
-      </c>
-      <c r="Y15">
-        <v>1</v>
-      </c>
-      <c r="AB15">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <v>0</v>
+      </c>
+      <c r="AE15">
+        <v>0</v>
       </c>
       <c r="AF15">
         <v>0</v>
       </c>
-      <c r="AG15">
-        <v>0</v>
-      </c>
-      <c r="AI15">
-        <v>0</v>
-      </c>
-      <c r="AJ15">
+      <c r="AN15">
         <v>0</v>
       </c>
       <c r="AO15">
         <v>0</v>
       </c>
-      <c r="AP15">
-        <v>0</v>
-      </c>
-      <c r="AX15">
-        <v>0</v>
-      </c>
-      <c r="AY15">
-        <v>0</v>
-      </c>
-      <c r="BA15">
-        <v>0</v>
-      </c>
-      <c r="BC15">
-        <v>0</v>
-      </c>
     </row>
-    <row r="16" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2248,19 +1871,19 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D16">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E16">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="H16">
         <v>219</v>
       </c>
       <c r="I16">
-        <v>81437</v>
+        <v>72090</v>
       </c>
       <c r="J16">
         <v>3</v>
@@ -2272,79 +1895,58 @@
         <v>1</v>
       </c>
       <c r="M16">
-        <v>2.2999999999999998</v>
+        <v>2.89</v>
       </c>
       <c r="N16">
-        <v>1.55E-2</v>
+        <v>4.6600000000000003E-2</v>
       </c>
       <c r="O16">
-        <v>5.03</v>
+        <v>4.95</v>
       </c>
       <c r="P16">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="Q16">
-        <v>138.4</v>
+        <v>0</v>
       </c>
       <c r="R16">
-        <v>0</v>
+        <v>19222</v>
       </c>
       <c r="S16">
-        <v>23246</v>
+        <v>1</v>
       </c>
       <c r="T16">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V16">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X16">
-        <v>1</v>
-      </c>
-      <c r="Y16">
-        <v>1</v>
-      </c>
-      <c r="AB16">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AA16">
+        <v>0</v>
+      </c>
+      <c r="AE16">
+        <v>0</v>
       </c>
       <c r="AF16">
         <v>0</v>
       </c>
-      <c r="AG16">
-        <v>0</v>
-      </c>
-      <c r="AI16">
-        <v>0</v>
-      </c>
-      <c r="AJ16">
+      <c r="AN16">
         <v>0</v>
       </c>
       <c r="AO16">
         <v>0</v>
       </c>
-      <c r="AP16">
-        <v>0</v>
-      </c>
-      <c r="AX16">
-        <v>0</v>
-      </c>
-      <c r="AY16">
-        <v>0</v>
-      </c>
-      <c r="BA16">
-        <v>0</v>
-      </c>
-      <c r="BC16">
-        <v>0</v>
-      </c>
     </row>
-    <row r="17" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2352,109 +1954,82 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D17">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E17">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="H17">
         <v>219</v>
       </c>
       <c r="I17">
-        <v>85728</v>
+        <v>73666</v>
       </c>
       <c r="J17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K17">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="L17">
         <v>1</v>
       </c>
       <c r="M17">
-        <v>1.79</v>
+        <v>2.89</v>
       </c>
       <c r="N17">
-        <v>7.1999999999999998E-3</v>
+        <v>0.22720000000000001</v>
       </c>
       <c r="O17">
-        <v>4.5</v>
+        <v>4.79</v>
       </c>
       <c r="P17">
-        <v>31</v>
+        <v>149</v>
       </c>
       <c r="Q17">
-        <v>100.89</v>
+        <v>0</v>
       </c>
       <c r="R17">
-        <v>0</v>
+        <v>19222</v>
       </c>
       <c r="S17">
-        <v>23246</v>
+        <v>1</v>
       </c>
       <c r="T17">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V17">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X17">
-        <v>1</v>
-      </c>
-      <c r="Y17">
-        <v>1</v>
-      </c>
-      <c r="AB17">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AA17">
+        <v>0</v>
+      </c>
+      <c r="AE17">
+        <v>0</v>
       </c>
       <c r="AF17">
         <v>0</v>
       </c>
-      <c r="AG17">
-        <v>0</v>
-      </c>
-      <c r="AI17">
-        <v>0</v>
-      </c>
-      <c r="AJ17">
-        <v>0</v>
-      </c>
-      <c r="AK17">
-        <v>8</v>
+      <c r="AN17">
+        <v>0</v>
       </c>
       <c r="AO17">
-        <v>1</v>
-      </c>
-      <c r="AP17">
-        <v>-1</v>
-      </c>
-      <c r="AQ17">
-        <v>14</v>
-      </c>
-      <c r="AX17">
-        <v>0</v>
-      </c>
-      <c r="AY17">
-        <v>0</v>
-      </c>
-      <c r="BA17">
-        <v>0</v>
-      </c>
-      <c r="BC17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2462,22 +2037,22 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D18">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E18">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="H18">
         <v>219</v>
       </c>
       <c r="I18">
-        <v>88096</v>
+        <v>74045</v>
       </c>
       <c r="J18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K18">
         <v>4</v>
@@ -2486,91 +2061,58 @@
         <v>1</v>
       </c>
       <c r="M18">
-        <v>2.94</v>
+        <v>2.77</v>
       </c>
       <c r="N18">
-        <v>6.6000000000000003E-2</v>
+        <v>0.20030000000000001</v>
       </c>
       <c r="O18">
-        <v>5.18</v>
+        <v>4.5599999999999996</v>
       </c>
       <c r="P18">
-        <v>23</v>
+        <v>89.99</v>
       </c>
       <c r="Q18">
-        <v>152.63</v>
+        <v>0</v>
       </c>
       <c r="R18">
-        <v>1</v>
+        <v>19222</v>
       </c>
       <c r="S18">
-        <v>23246</v>
+        <v>1</v>
       </c>
       <c r="T18">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V18">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X18">
-        <v>1</v>
-      </c>
-      <c r="Y18">
-        <v>1</v>
-      </c>
-      <c r="AB18">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AA18">
+        <v>0</v>
+      </c>
+      <c r="AE18">
+        <v>0</v>
       </c>
       <c r="AF18">
         <v>0</v>
       </c>
-      <c r="AG18">
-        <v>0</v>
-      </c>
-      <c r="AH18">
-        <v>5</v>
-      </c>
-      <c r="AI18">
-        <v>0</v>
-      </c>
-      <c r="AJ18">
-        <v>0</v>
-      </c>
-      <c r="AK18">
-        <v>5</v>
+      <c r="AN18">
+        <v>0</v>
       </c>
       <c r="AO18">
-        <v>1</v>
-      </c>
-      <c r="AP18">
-        <v>0</v>
-      </c>
-      <c r="AQ18">
-        <v>5</v>
-      </c>
-      <c r="AX18">
-        <v>0</v>
-      </c>
-      <c r="AY18">
-        <v>0</v>
-      </c>
-      <c r="AZ18">
-        <v>15</v>
-      </c>
-      <c r="BA18">
-        <v>0</v>
-      </c>
-      <c r="BC18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2578,97 +2120,76 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D19">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E19">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="H19">
         <v>219</v>
       </c>
       <c r="I19">
-        <v>88127</v>
+        <v>78599</v>
       </c>
       <c r="J19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K19">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="L19">
         <v>1</v>
       </c>
       <c r="M19">
-        <v>1.39</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="N19">
-        <v>3.8E-3</v>
+        <v>8.9499999999999996E-2</v>
       </c>
       <c r="O19">
-        <v>4.8</v>
+        <v>5.0599999999999996</v>
       </c>
       <c r="P19">
-        <v>36</v>
+        <v>158.87</v>
       </c>
       <c r="Q19">
-        <v>138.4</v>
+        <v>0</v>
       </c>
       <c r="R19">
-        <v>0</v>
+        <v>19222</v>
       </c>
       <c r="S19">
-        <v>23246</v>
+        <v>1</v>
       </c>
       <c r="T19">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V19">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X19">
-        <v>1</v>
-      </c>
-      <c r="Y19">
-        <v>1</v>
-      </c>
-      <c r="AB19">
-        <v>1</v>
-      </c>
-      <c r="AF19">
-        <v>0</v>
-      </c>
-      <c r="AG19">
-        <v>0</v>
-      </c>
-      <c r="AI19">
-        <v>0</v>
-      </c>
-      <c r="AJ19">
-        <v>0</v>
-      </c>
-      <c r="AX19">
-        <v>0</v>
-      </c>
-      <c r="AY19">
-        <v>0</v>
-      </c>
-      <c r="BA19">
-        <v>0</v>
-      </c>
-      <c r="BC19">
+        <v>0</v>
+      </c>
+      <c r="AA19">
+        <v>0</v>
+      </c>
+      <c r="AN19">
+        <v>0</v>
+      </c>
+      <c r="AO19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2676,25 +2197,25 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D20">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E20">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="H20">
         <v>219</v>
       </c>
       <c r="I20">
-        <v>88218</v>
+        <v>82231</v>
       </c>
       <c r="J20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K20">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="L20">
         <v>1</v>
@@ -2703,76 +2224,55 @@
         <v>2.77</v>
       </c>
       <c r="N20">
-        <v>0.12659999999999999</v>
+        <v>0.20899999999999999</v>
       </c>
       <c r="O20">
-        <v>4.9800000000000004</v>
+        <v>4.92</v>
       </c>
       <c r="P20">
-        <v>8</v>
+        <v>104</v>
       </c>
       <c r="Q20">
-        <v>115.12</v>
+        <v>0</v>
       </c>
       <c r="R20">
-        <v>0</v>
+        <v>19222</v>
       </c>
       <c r="S20">
-        <v>23246</v>
+        <v>1</v>
       </c>
       <c r="T20">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V20">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X20">
-        <v>1</v>
-      </c>
-      <c r="Y20">
-        <v>1</v>
-      </c>
-      <c r="AB20">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AA20">
+        <v>0</v>
+      </c>
+      <c r="AE20">
+        <v>0</v>
       </c>
       <c r="AF20">
         <v>0</v>
       </c>
-      <c r="AG20">
-        <v>0</v>
-      </c>
-      <c r="AI20">
-        <v>0</v>
-      </c>
-      <c r="AJ20">
+      <c r="AN20">
         <v>0</v>
       </c>
       <c r="AO20">
         <v>0</v>
       </c>
-      <c r="AP20">
-        <v>-1</v>
-      </c>
-      <c r="AX20">
-        <v>0</v>
-      </c>
-      <c r="AY20">
-        <v>0</v>
-      </c>
-      <c r="BA20">
-        <v>0</v>
-      </c>
-      <c r="BC20">
-        <v>0</v>
-      </c>
     </row>
-    <row r="21" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2780,103 +2280,76 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D21">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E21">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="H21">
         <v>219</v>
       </c>
       <c r="I21">
-        <v>89073</v>
+        <v>89466</v>
       </c>
       <c r="J21">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M21">
         <v>2.08</v>
       </c>
       <c r="N21">
-        <v>1.4999999999999999E-2</v>
+        <v>7.7799999999999994E-2</v>
       </c>
       <c r="O21">
-        <v>5.28</v>
+        <v>4.3099999999999996</v>
       </c>
       <c r="P21">
-        <v>6</v>
+        <v>58.57</v>
       </c>
       <c r="Q21">
-        <v>191.44</v>
+        <v>0</v>
       </c>
       <c r="R21">
-        <v>0</v>
+        <v>19222</v>
       </c>
       <c r="S21">
-        <v>23246</v>
+        <v>1</v>
       </c>
       <c r="T21">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V21">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X21">
-        <v>1</v>
-      </c>
-      <c r="Y21">
-        <v>1</v>
-      </c>
-      <c r="AB21">
-        <v>1</v>
-      </c>
-      <c r="AI21">
-        <v>0</v>
-      </c>
-      <c r="AJ21">
-        <v>0</v>
-      </c>
-      <c r="AK21">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="AA21">
+        <v>0</v>
+      </c>
+      <c r="AN21">
+        <v>0</v>
       </c>
       <c r="AO21">
         <v>0</v>
       </c>
-      <c r="AP21">
-        <v>0</v>
-      </c>
-      <c r="AX21">
-        <v>0</v>
-      </c>
-      <c r="AY21">
-        <v>0</v>
-      </c>
-      <c r="AZ21">
-        <v>5</v>
-      </c>
-      <c r="BA21">
-        <v>0</v>
-      </c>
-      <c r="BC21">
-        <v>0</v>
-      </c>
     </row>
-    <row r="22" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2884,103 +2357,82 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D22">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E22">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="H22">
         <v>219</v>
       </c>
       <c r="I22">
-        <v>95166</v>
+        <v>90385</v>
       </c>
       <c r="J22">
         <v>3</v>
       </c>
       <c r="K22">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="L22">
         <v>1</v>
       </c>
       <c r="M22">
-        <v>2.71</v>
+        <v>2.77</v>
       </c>
       <c r="N22">
-        <v>3.5900000000000001E-2</v>
+        <v>5.6899999999999999E-2</v>
       </c>
       <c r="O22">
-        <v>4.71</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="P22">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="Q22">
-        <v>122.88</v>
+        <v>0</v>
       </c>
       <c r="R22">
-        <v>0</v>
+        <v>19222</v>
       </c>
       <c r="S22">
-        <v>23246</v>
+        <v>1</v>
       </c>
       <c r="T22">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V22">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X22">
-        <v>1</v>
-      </c>
-      <c r="Y22">
-        <v>1</v>
-      </c>
-      <c r="AB22">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AA22">
+        <v>0</v>
+      </c>
+      <c r="AE22">
+        <v>0</v>
       </c>
       <c r="AF22">
         <v>0</v>
       </c>
-      <c r="AG22">
-        <v>0</v>
-      </c>
-      <c r="AH22">
-        <v>12</v>
-      </c>
-      <c r="AI22">
-        <v>0</v>
-      </c>
-      <c r="AJ22">
-        <v>0</v>
-      </c>
-      <c r="AK22">
-        <v>6</v>
-      </c>
-      <c r="AX22">
-        <v>0</v>
-      </c>
-      <c r="AY22">
-        <v>0</v>
-      </c>
-      <c r="BA22">
-        <v>0</v>
-      </c>
-      <c r="BC22">
+      <c r="AN22">
+        <v>0</v>
+      </c>
+      <c r="AO22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2988,100 +2440,88 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D23">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E23">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="H23">
         <v>219</v>
       </c>
       <c r="I23">
-        <v>95307</v>
+        <v>94729</v>
       </c>
       <c r="J23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K23">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="L23">
         <v>1</v>
       </c>
       <c r="M23">
-        <v>2.4</v>
+        <v>2.83</v>
       </c>
       <c r="N23">
-        <v>0.1149</v>
+        <v>0.23949999999999999</v>
       </c>
       <c r="O23">
-        <v>4.93</v>
+        <v>4.82</v>
       </c>
       <c r="P23">
-        <v>1</v>
+        <v>139</v>
       </c>
       <c r="Q23">
-        <v>139.69999999999999</v>
+        <v>0</v>
       </c>
       <c r="R23">
-        <v>0</v>
+        <v>19222</v>
       </c>
       <c r="S23">
-        <v>23246</v>
+        <v>1</v>
       </c>
       <c r="T23">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V23">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X23">
-        <v>1</v>
-      </c>
-      <c r="Y23">
-        <v>1</v>
-      </c>
-      <c r="AB23">
-        <v>1</v>
-      </c>
-      <c r="AI23">
-        <v>0</v>
-      </c>
-      <c r="AJ23">
-        <v>0</v>
-      </c>
-      <c r="AK23">
-        <v>29</v>
+        <v>0</v>
+      </c>
+      <c r="AA23">
+        <v>0</v>
+      </c>
+      <c r="AE23">
+        <v>0</v>
+      </c>
+      <c r="AF23">
+        <v>0</v>
+      </c>
+      <c r="AG23">
+        <v>17</v>
+      </c>
+      <c r="AN23">
+        <v>0</v>
+      </c>
+      <c r="AO23">
+        <v>0</v>
       </c>
       <c r="AP23">
-        <v>1</v>
-      </c>
-      <c r="AX23">
-        <v>-1</v>
-      </c>
-      <c r="AY23">
-        <v>0</v>
-      </c>
-      <c r="AZ23">
-        <v>27</v>
-      </c>
-      <c r="BA23">
-        <v>0</v>
-      </c>
-      <c r="BC23">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -3089,22 +2529,22 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D24">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E24">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="H24">
         <v>219</v>
       </c>
       <c r="I24">
-        <v>97247</v>
+        <v>95031</v>
       </c>
       <c r="J24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K24">
         <v>3.5</v>
@@ -3116,85 +2556,55 @@
         <v>2.83</v>
       </c>
       <c r="N24">
-        <v>1.4500000000000001E-2</v>
+        <v>9.0800000000000006E-2</v>
       </c>
       <c r="O24">
-        <v>4.68</v>
+        <v>4.5</v>
       </c>
       <c r="P24">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="Q24">
-        <v>115.12</v>
+        <v>0</v>
       </c>
       <c r="R24">
-        <v>0</v>
+        <v>19222</v>
       </c>
       <c r="S24">
-        <v>23246</v>
+        <v>1</v>
       </c>
       <c r="T24">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V24">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X24">
-        <v>1</v>
-      </c>
-      <c r="Y24">
-        <v>1</v>
-      </c>
-      <c r="AB24">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AA24">
+        <v>0</v>
+      </c>
+      <c r="AE24">
+        <v>0</v>
       </c>
       <c r="AF24">
         <v>0</v>
       </c>
-      <c r="AG24">
-        <v>0</v>
-      </c>
-      <c r="AI24">
-        <v>0</v>
-      </c>
-      <c r="AJ24">
-        <v>0</v>
-      </c>
-      <c r="AK24">
-        <v>5</v>
+      <c r="AN24">
+        <v>0</v>
       </c>
       <c r="AO24">
-        <v>1</v>
-      </c>
-      <c r="AP24">
-        <v>1</v>
-      </c>
-      <c r="AQ24">
-        <v>9</v>
-      </c>
-      <c r="AX24">
-        <v>-1</v>
-      </c>
-      <c r="AY24">
-        <v>0</v>
-      </c>
-      <c r="AZ24">
-        <v>5</v>
-      </c>
-      <c r="BA24">
-        <v>0</v>
-      </c>
-      <c r="BC24">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -3202,115 +2612,85 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D25">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E25">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="H25">
         <v>219</v>
       </c>
       <c r="I25">
-        <v>107872</v>
+        <v>99484</v>
       </c>
       <c r="J25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K25">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="L25">
         <v>1</v>
       </c>
       <c r="M25">
-        <v>2.71</v>
+        <v>2.4</v>
       </c>
       <c r="N25">
-        <v>4.65E-2</v>
+        <v>0.21820000000000001</v>
       </c>
       <c r="O25">
-        <v>4.4400000000000004</v>
+        <v>4.54</v>
       </c>
       <c r="P25">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="Q25">
-        <v>128.06</v>
+        <v>1</v>
       </c>
       <c r="R25">
-        <v>0</v>
+        <v>19222</v>
       </c>
       <c r="S25">
-        <v>23246</v>
+        <v>1</v>
       </c>
       <c r="T25">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V25">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X25">
-        <v>1</v>
-      </c>
-      <c r="Y25">
-        <v>1</v>
-      </c>
-      <c r="AB25">
+        <v>0</v>
+      </c>
+      <c r="AA25">
+        <v>0</v>
+      </c>
+      <c r="AE25">
         <v>1</v>
       </c>
       <c r="AF25">
         <v>0</v>
       </c>
       <c r="AG25">
-        <v>0</v>
-      </c>
-      <c r="AH25">
-        <v>23</v>
-      </c>
-      <c r="AI25">
-        <v>0</v>
-      </c>
-      <c r="AJ25">
-        <v>0</v>
-      </c>
-      <c r="AK25">
-        <v>10</v>
+        <v>2</v>
+      </c>
+      <c r="AN25">
+        <v>0</v>
       </c>
       <c r="AO25">
-        <v>1</v>
-      </c>
-      <c r="AP25">
-        <v>-1</v>
-      </c>
-      <c r="AQ25">
-        <v>3</v>
-      </c>
-      <c r="AX25">
-        <v>0</v>
-      </c>
-      <c r="AY25">
-        <v>0</v>
-      </c>
-      <c r="AZ25">
-        <v>14</v>
-      </c>
-      <c r="BA25">
-        <v>0</v>
-      </c>
-      <c r="BC25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -3318,19 +2698,19 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D26">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E26">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="H26">
         <v>219</v>
       </c>
       <c r="I26">
-        <v>111000</v>
+        <v>123675</v>
       </c>
       <c r="J26">
         <v>3</v>
@@ -3342,79 +2722,58 @@
         <v>1</v>
       </c>
       <c r="M26">
-        <v>2.2000000000000002</v>
+        <v>2.83</v>
       </c>
       <c r="N26">
-        <v>1.6400000000000001E-2</v>
+        <v>0.2303</v>
       </c>
       <c r="O26">
-        <v>5.0199999999999996</v>
+        <v>4.66</v>
       </c>
       <c r="P26">
-        <v>24</v>
+        <v>109</v>
       </c>
       <c r="Q26">
-        <v>181.09</v>
+        <v>0</v>
       </c>
       <c r="R26">
-        <v>0</v>
+        <v>19222</v>
       </c>
       <c r="S26">
-        <v>23246</v>
+        <v>1</v>
       </c>
       <c r="T26">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V26">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X26">
-        <v>1</v>
-      </c>
-      <c r="Y26">
-        <v>1</v>
-      </c>
-      <c r="AB26">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AA26">
+        <v>0</v>
+      </c>
+      <c r="AE26">
+        <v>0</v>
       </c>
       <c r="AF26">
         <v>0</v>
       </c>
-      <c r="AG26">
-        <v>0</v>
-      </c>
-      <c r="AI26">
-        <v>0</v>
-      </c>
-      <c r="AJ26">
+      <c r="AN26">
         <v>0</v>
       </c>
       <c r="AO26">
         <v>0</v>
       </c>
-      <c r="AP26">
-        <v>0</v>
-      </c>
-      <c r="AX26">
-        <v>0</v>
-      </c>
-      <c r="AY26">
-        <v>0</v>
-      </c>
-      <c r="BA26">
-        <v>0</v>
-      </c>
-      <c r="BC26">
-        <v>0</v>
-      </c>
     </row>
-    <row r="27" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -3422,97 +2781,88 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D27">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E27">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="H27">
         <v>219</v>
       </c>
       <c r="I27">
-        <v>111106</v>
+        <v>128085</v>
       </c>
       <c r="J27">
+        <v>2</v>
+      </c>
+      <c r="K27">
         <v>3</v>
       </c>
-      <c r="K27">
-        <v>2.5</v>
-      </c>
       <c r="L27">
         <v>1</v>
       </c>
       <c r="M27">
-        <v>0.69</v>
+        <v>2.4</v>
       </c>
       <c r="N27">
-        <v>7.1000000000000004E-3</v>
+        <v>5.1799999999999999E-2</v>
       </c>
       <c r="O27">
-        <v>4.67</v>
+        <v>4.1900000000000004</v>
       </c>
       <c r="P27">
-        <v>37</v>
+        <v>47.97</v>
       </c>
       <c r="Q27">
-        <v>120.29</v>
+        <v>1</v>
       </c>
       <c r="R27">
-        <v>0</v>
+        <v>19222</v>
       </c>
       <c r="S27">
-        <v>23246</v>
+        <v>1</v>
       </c>
       <c r="T27">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V27">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X27">
-        <v>1</v>
-      </c>
-      <c r="Y27">
-        <v>1</v>
-      </c>
-      <c r="AB27">
+        <v>0</v>
+      </c>
+      <c r="AA27">
+        <v>0</v>
+      </c>
+      <c r="AE27">
         <v>1</v>
       </c>
       <c r="AF27">
         <v>0</v>
       </c>
       <c r="AG27">
-        <v>0</v>
-      </c>
-      <c r="AI27">
-        <v>0</v>
-      </c>
-      <c r="AJ27">
-        <v>0</v>
-      </c>
-      <c r="AX27">
-        <v>0</v>
-      </c>
-      <c r="AY27">
-        <v>0</v>
-      </c>
-      <c r="BA27">
-        <v>0</v>
-      </c>
-      <c r="BC27">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="AN27">
+        <v>1</v>
+      </c>
+      <c r="AO27">
+        <v>0</v>
+      </c>
+      <c r="AP27">
+        <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -3520,82 +2870,82 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D28">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E28">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="H28">
         <v>219</v>
       </c>
       <c r="I28">
-        <v>114766</v>
+        <v>128871</v>
       </c>
       <c r="J28">
         <v>2</v>
       </c>
       <c r="K28">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="L28">
         <v>1</v>
       </c>
       <c r="M28">
-        <v>1.61</v>
+        <v>2.56</v>
       </c>
       <c r="N28">
-        <v>5.1999999999999998E-3</v>
+        <v>4.6899999999999997E-2</v>
       </c>
       <c r="O28">
-        <v>4.67</v>
+        <v>4.21</v>
       </c>
       <c r="P28">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="Q28">
-        <v>104.77</v>
+        <v>0</v>
       </c>
       <c r="R28">
-        <v>0</v>
+        <v>19222</v>
       </c>
       <c r="S28">
-        <v>23246</v>
+        <v>1</v>
       </c>
       <c r="T28">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V28">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X28">
-        <v>1</v>
-      </c>
-      <c r="Y28">
-        <v>1</v>
-      </c>
-      <c r="AB28">
-        <v>1</v>
-      </c>
-      <c r="AP28">
-        <v>-1</v>
-      </c>
-      <c r="BA28">
-        <v>0</v>
-      </c>
-      <c r="BC28">
+        <v>0</v>
+      </c>
+      <c r="AA28">
+        <v>0</v>
+      </c>
+      <c r="AE28">
+        <v>0</v>
+      </c>
+      <c r="AF28">
+        <v>0</v>
+      </c>
+      <c r="AN28">
+        <v>0</v>
+      </c>
+      <c r="AO28">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -3603,99 +2953,149 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D29">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E29">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="H29">
         <v>219</v>
       </c>
       <c r="I29">
-        <v>122844</v>
+        <v>134992</v>
       </c>
       <c r="J29">
+        <v>2</v>
+      </c>
+      <c r="K29">
+        <v>5</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <v>3.04</v>
+      </c>
+      <c r="N29">
+        <v>0.1401</v>
+      </c>
+      <c r="O29">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="P29">
+        <v>119</v>
+      </c>
+      <c r="Q29">
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <v>19222</v>
+      </c>
+      <c r="S29">
+        <v>1</v>
+      </c>
+      <c r="T29">
+        <v>10</v>
+      </c>
+      <c r="U29">
+        <v>2</v>
+      </c>
+      <c r="V29">
+        <v>0</v>
+      </c>
+      <c r="W29">
+        <v>1</v>
+      </c>
+      <c r="X29">
+        <v>0</v>
+      </c>
+      <c r="AA29">
+        <v>0</v>
+      </c>
+      <c r="AE29">
+        <v>0</v>
+      </c>
+      <c r="AF29">
+        <v>0</v>
+      </c>
+      <c r="AN29">
+        <v>0</v>
+      </c>
+      <c r="AO29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30">
+        <v>24</v>
+      </c>
+      <c r="E30">
+        <v>216</v>
+      </c>
+      <c r="H30">
+        <v>219</v>
+      </c>
+      <c r="I30">
+        <v>139162</v>
+      </c>
+      <c r="J30">
         <v>3</v>
       </c>
-      <c r="K29">
+      <c r="K30">
         <v>4.5</v>
       </c>
-      <c r="L29">
-        <v>1</v>
-      </c>
-      <c r="M29">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="N29">
-        <v>3.2000000000000002E-3</v>
-      </c>
-      <c r="O29">
-        <v>5.46</v>
-      </c>
-      <c r="P29">
-        <v>29</v>
-      </c>
-      <c r="Q29">
-        <v>190.14</v>
-      </c>
-      <c r="R29">
-        <v>0</v>
-      </c>
-      <c r="S29">
-        <v>23246</v>
-      </c>
-      <c r="T29">
-        <v>1</v>
-      </c>
-      <c r="U29">
-        <v>0</v>
-      </c>
-      <c r="V29">
-        <v>4</v>
-      </c>
-      <c r="W29">
-        <v>0</v>
-      </c>
-      <c r="X29">
-        <v>1</v>
-      </c>
-      <c r="Y29">
-        <v>1</v>
-      </c>
-      <c r="AB29">
-        <v>1</v>
-      </c>
-      <c r="AF29">
-        <v>0</v>
-      </c>
-      <c r="AG29">
-        <v>0</v>
-      </c>
-      <c r="AI29">
-        <v>0</v>
-      </c>
-      <c r="AJ29">
-        <v>0</v>
-      </c>
-      <c r="AO29">
-        <v>0</v>
-      </c>
-      <c r="AP29">
-        <v>0</v>
-      </c>
-      <c r="AX29">
-        <v>0</v>
-      </c>
-      <c r="AY29">
-        <v>0</v>
-      </c>
-      <c r="BA29">
-        <v>0</v>
-      </c>
-      <c r="BC29">
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N30">
+        <v>6.1800000000000001E-2</v>
+      </c>
+      <c r="O30">
+        <v>5.03</v>
+      </c>
+      <c r="P30">
+        <v>169</v>
+      </c>
+      <c r="Q30">
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <v>19222</v>
+      </c>
+      <c r="S30">
+        <v>1</v>
+      </c>
+      <c r="T30">
+        <v>10</v>
+      </c>
+      <c r="U30">
+        <v>2</v>
+      </c>
+      <c r="V30">
+        <v>0</v>
+      </c>
+      <c r="W30">
+        <v>1</v>
+      </c>
+      <c r="X30">
+        <v>0</v>
+      </c>
+      <c r="AA30">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
made function to drop cols with more than x% of data missing
</commit_message>
<xml_diff>
--- a/EDA/srch_id_1.xlsx
+++ b/EDA/srch_id_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c98b824bff33be6/MSc. Artificial Intelligence VU/MSc. AI Year 1/Data Mining Techniques/Assignment 2/new_clone/dmt-2/EDA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_371659DF44BC10E5DA170B6CA376D07750523176" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{639E8656-96A6-44BC-8BAB-A9F4622CF603}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_371659DF44BC10E5DA170B6CA376D07750523176" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07F27AE7-881E-4C17-B78E-771E8A0633B4}"/>
   <bookViews>
-    <workbookView xWindow="1812" yWindow="1812" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="new_sheet" sheetId="1" r:id="rId1"/>
@@ -577,12 +577,61 @@
   <dimension ref="A1:AY30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13:K27"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="9" max="9" width="18.21875" customWidth="1"/>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="23" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="22.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:51" x14ac:dyDescent="0.3">

</xml_diff>